<commit_message>
Update Leave Card 1/15/2024 3:59 PM
</commit_message>
<xml_diff>
--- a/1-TEMPALTE LEAVE CARD.xlsx
+++ b/1-TEMPALTE LEAVE CARD.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\dole-pc\Users\DOLE\Desktop\LEAVE-CARD\JOBCON\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\dole-pc\Users\DOLE\Desktop\LEAVE-CARD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D70463FA-B88F-443E-8385-8D73733CF93C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B66F5BFE-531A-437F-89B8-9F7C31D17B8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{2C4B9B69-0AD3-46D4-A495-D1BDE1D16EC6}"/>
   </bookViews>
@@ -2942,8 +2942,8 @@
   </sheetPr>
   <dimension ref="A2:K130"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3576" topLeftCell="A7" activePane="bottomLeft"/>
+    <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="5520" topLeftCell="A34" activePane="bottomLeft"/>
       <selection activeCell="B4" sqref="B4:C4"/>
       <selection pane="bottomLeft" activeCell="N14" sqref="N14"/>
     </sheetView>
@@ -5069,7 +5069,7 @@
     <mergeCell ref="F3:G3"/>
     <mergeCell ref="F4:G4"/>
   </mergeCells>
-  <dataValidations count="2">
+  <dataValidations disablePrompts="1" count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:G2" xr:uid="{3C67B38A-DE91-4BA1-85D0-F5C61D6395E6}">
       <formula1>"1 - Married (and not separated), 2 - Widowed (including living common law), 3 - Separated (including living common law), 4 - Divorced (including living common law), 5 - Single (including living common law)"</formula1>
     </dataValidation>
@@ -5086,8 +5086,8 @@
     <oddFooter>&amp;L
 PREPARED BY: ___________________
 DATE: &amp;D, &amp;T&amp;C
-CERTIFIED CORRECT BY: &amp;UALMA A. MALABANAN&amp;U
-                                   HRMO&amp;RPage &amp;P of &amp;N</oddFooter>
+CERTIFIED CORRECT BY: &amp;UNANETTE B. SUSA&amp;U
+                                            OIC - HRMO&amp;RPage &amp;P of &amp;N</oddFooter>
   </headerFooter>
   <tableParts count="1">
     <tablePart r:id="rId2"/>

</xml_diff>

<commit_message>
update leave card 2/7/2024 4:36pm
</commit_message>
<xml_diff>
--- a/1-TEMPALTE LEAVE CARD.xlsx
+++ b/1-TEMPALTE LEAVE CARD.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
-  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\dole-pc\Users\DOLE\Desktop\LEAVE-CARD\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DOLE\Desktop\LEAVE-CARD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B66F5BFE-531A-437F-89B8-9F7C31D17B8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{2C4B9B69-0AD3-46D4-A495-D1BDE1D16EC6}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="INSTRUCTION" sheetId="4" r:id="rId1"/>
@@ -25,7 +24,7 @@
     <definedName name="BALANCE_1">Table1[[#Headers],[BALANCE]]</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="1">Sheet1!$1:$9</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -169,7 +168,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="4">
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="mm/dd/yy;@"/>
@@ -594,7 +593,6 @@
         <sz val="11"/>
         <color theme="1"/>
         <name val="Calibri"/>
-        <family val="2"/>
         <scheme val="minor"/>
       </font>
       <numFmt numFmtId="164" formatCode="0.000"/>
@@ -669,7 +667,6 @@
         <sz val="11"/>
         <color theme="1"/>
         <name val="Calibri"/>
-        <family val="2"/>
         <scheme val="minor"/>
       </font>
       <numFmt numFmtId="164" formatCode="0.000"/>
@@ -737,7 +734,6 @@
         <sz val="11"/>
         <color theme="1"/>
         <name val="Calibri"/>
-        <family val="2"/>
         <scheme val="minor"/>
       </font>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -979,7 +975,6 @@
         <sz val="11"/>
         <color theme="1"/>
         <name val="Calibri"/>
-        <family val="2"/>
         <scheme val="minor"/>
       </font>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -1027,7 +1022,7 @@
         <xdr:cNvPr id="7" name="Picture 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3B5D8F3C-4FD5-4318-83F6-163B56792B3A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{3B5D8F3C-4FD5-4318-83F6-163B56792B3A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1070,7 +1065,7 @@
         <xdr:cNvPr id="5" name="TextBox 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A0BAE224-67DC-A2F7-0A1F-28CB86DFB7CA}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{A0BAE224-67DC-A2F7-0A1F-28CB86DFB7CA}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1134,7 +1129,7 @@
         <xdr:cNvPr id="4" name="Arrow: Left 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7243AC54-FD55-C7CF-DEF3-E45E6F99CAA1}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{7243AC54-FD55-C7CF-DEF3-E45E6F99CAA1}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1194,7 +1189,7 @@
         <xdr:cNvPr id="8" name="Oval 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6CEC4AD9-D5D6-0CFD-8D82-CC23F90E3707}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{6CEC4AD9-D5D6-0CFD-8D82-CC23F90E3707}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1260,7 +1255,7 @@
         <xdr:cNvPr id="9" name="Arrow: Left-Right 8">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EAE8B24D-B9B9-4AB0-AE94-782594B55A03}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{EAE8B24D-B9B9-4AB0-AE94-782594B55A03}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1323,7 +1318,7 @@
         <xdr:cNvPr id="10" name="TextBox 9">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D163C4F0-3D7F-3E52-4B17-0D29F1241915}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{D163C4F0-3D7F-3E52-4B17-0D29F1241915}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1421,7 +1416,7 @@
         <xdr:cNvPr id="14" name="Straight Arrow Connector 13">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{642CA079-93A1-34E3-CEF5-F7D33015D895}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{642CA079-93A1-34E3-CEF5-F7D33015D895}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1480,7 +1475,7 @@
         <xdr:cNvPr id="19" name="TextBox 18">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{784FECEA-1780-3E7F-7EBB-9F8254797C91}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{784FECEA-1780-3E7F-7EBB-9F8254797C91}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1545,7 +1540,7 @@
         <xdr:cNvPr id="20" name="Picture 19">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5DCCE859-255F-F039-E92D-1510F02C6167}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{5DCCE859-255F-F039-E92D-1510F02C6167}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1588,7 +1583,7 @@
         <xdr:cNvPr id="21" name="TextBox 20">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0A7AA7C6-9540-EB37-E3D2-9A2A68BD6824}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{0A7AA7C6-9540-EB37-E3D2-9A2A68BD6824}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1663,7 +1658,7 @@
         <xdr:cNvPr id="22" name="TextBox 21">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F1674299-9801-A253-3871-18715F4FF740}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{F1674299-9801-A253-3871-18715F4FF740}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1849,7 +1844,7 @@
         <xdr:cNvPr id="23" name="Oval 22">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{66C92862-99CA-461F-932E-30DFD0874402}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{66C92862-99CA-461F-932E-30DFD0874402}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1915,7 +1910,7 @@
         <xdr:cNvPr id="24" name="Straight Arrow Connector 23">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FD20A152-8288-4C69-BE76-AD8E41A960CE}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{FD20A152-8288-4C69-BE76-AD8E41A960CE}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1973,7 +1968,7 @@
         <xdr:cNvPr id="26" name="Oval 25">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EE7E56BE-0B3E-4110-A5A9-44C888A46B90}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{EE7E56BE-0B3E-4110-A5A9-44C888A46B90}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2039,7 +2034,7 @@
         <xdr:cNvPr id="27" name="Straight Arrow Connector 26">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C33E41C1-1592-4272-A561-4833666913C5}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{C33E41C1-1592-4272-A561-4833666913C5}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2095,7 +2090,7 @@
         <xdr:cNvPr id="30" name="TextBox 29">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6C655B57-0D66-4740-B73E-75D1E106F99A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{6C655B57-0D66-4740-B73E-75D1E106F99A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2170,7 +2165,7 @@
         <xdr:cNvPr id="31" name="Picture 30">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0284C105-1E11-4529-B509-D655B8C5279A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{0284C105-1E11-4529-B509-D655B8C5279A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2213,7 +2208,7 @@
         <xdr:cNvPr id="32" name="Oval 31">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E73E9A40-2B3C-47DC-9C07-7C65795CE0A2}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{E73E9A40-2B3C-47DC-9C07-7C65795CE0A2}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2279,7 +2274,7 @@
         <xdr:cNvPr id="33" name="Straight Arrow Connector 32">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{32002197-8137-42BA-B3E7-2690738DB64B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{32002197-8137-42BA-B3E7-2690738DB64B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2335,7 +2330,7 @@
         <xdr:cNvPr id="34" name="TextBox 33">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A781E01A-37B6-4259-9759-556FE6893D51}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{A781E01A-37B6-4259-9759-556FE6893D51}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2433,7 +2428,7 @@
         <xdr:cNvPr id="2" name="Rectangle 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C99D8E5F-2D60-FF91-2593-A29CC276458B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{C99D8E5F-2D60-FF91-2593-A29CC276458B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2496,7 +2491,7 @@
         <xdr:cNvPr id="3" name="Rectangle 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D7E6A331-FC2C-4EF9-8F5B-65908D453D1C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{D7E6A331-FC2C-4EF9-8F5B-65908D453D1C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2545,7 +2540,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Sheet1"/>
@@ -2562,25 +2557,25 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{1D52DCCA-84C7-4E23-9F01-BAD20F9E44D8}" name="Table1" displayName="Table1" ref="A8:K130" totalsRowShown="0" headerRowDxfId="24" headerRowBorderDxfId="23" tableBorderDxfId="22" totalsRowBorderDxfId="21">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A8:K117" totalsRowShown="0" headerRowDxfId="24" headerRowBorderDxfId="23" tableBorderDxfId="22" totalsRowBorderDxfId="21">
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{29298656-164E-44DD-A190-558D78410746}" name="PERIOD" dataDxfId="20"/>
-    <tableColumn id="2" xr3:uid="{653A013C-2253-41B2-B51E-E0CEE6FCA4B9}" name="PARTICULARS" dataDxfId="19"/>
-    <tableColumn id="3" xr3:uid="{23618FA7-8FE1-47F3-A791-7E4F2612427B}" name="EARNED" dataDxfId="18"/>
-    <tableColumn id="4" xr3:uid="{BA6D2C36-5CF4-40D7-AFDD-218AEBB26721}" name="Absence Undertime W/ Pay" dataDxfId="17"/>
-    <tableColumn id="5" xr3:uid="{44B79BA7-06A4-4888-BFE5-96396FB13C9E}" name="BALANCE" dataDxfId="16">
+    <tableColumn id="1" name="PERIOD" dataDxfId="20"/>
+    <tableColumn id="2" name="PARTICULARS" dataDxfId="19"/>
+    <tableColumn id="3" name="EARNED" dataDxfId="18"/>
+    <tableColumn id="4" name="Absence Undertime W/ Pay" dataDxfId="17"/>
+    <tableColumn id="5" name="BALANCE" dataDxfId="16">
       <calculatedColumnFormula>SUM(Table1[EARNED])-SUM(Table1[Absence Undertime W/ Pay])+CONVERTION!$A$3</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{1A20B288-1D72-4858-B3C2-871EB9CF011E}" name="Absence Undertime W/O Pay" dataDxfId="15"/>
-    <tableColumn id="7" xr3:uid="{16E84B2D-53AC-4AEA-B1BC-1BC1E2E9B51B}" name="EARNED " dataDxfId="14">
+    <tableColumn id="6" name="Absence Undertime W/O Pay" dataDxfId="15"/>
+    <tableColumn id="7" name="EARNED " dataDxfId="14">
       <calculatedColumnFormula>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{A10DEDBF-F571-4518-A832-0B75654FC984}" name="Absence Undertime  W/ Pay" dataDxfId="13"/>
-    <tableColumn id="9" xr3:uid="{9E225A68-4AC2-420E-B4D1-1378612CB5CD}" name="BALANCE " dataDxfId="12">
+    <tableColumn id="8" name="Absence Undertime  W/ Pay" dataDxfId="13"/>
+    <tableColumn id="9" name="BALANCE " dataDxfId="12">
       <calculatedColumnFormula>SUM(Table1[[EARNED ]])-SUM(Table1[Absence Undertime  W/ Pay])+CONVERTION!$B$3</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{715FA023-3759-440B-8D8E-42D3E30EC36F}" name="Absence Undertime  W/O Pay" dataDxfId="11"/>
-    <tableColumn id="11" xr3:uid="{7E55BDC4-4FFC-4009-94E5-7F3F3565D56A}" name="REMARKS" dataDxfId="10"/>
+    <tableColumn id="10" name="Absence Undertime  W/O Pay" dataDxfId="11"/>
+    <tableColumn id="11" name="REMARKS" dataDxfId="10"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -2592,13 +2587,13 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{CB44E398-F318-4683-B466-030B39F69924}" name="Table2" displayName="Table2" ref="D2:G3" totalsRowShown="0" headerRowDxfId="9" headerRowBorderDxfId="8" tableBorderDxfId="7" totalsRowBorderDxfId="6">
-  <autoFilter ref="D2:G3" xr:uid="{CB44E398-F318-4683-B466-030B39F69924}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="D2:G3" totalsRowShown="0" headerRowDxfId="9" headerRowBorderDxfId="8" tableBorderDxfId="7" totalsRowBorderDxfId="6">
+  <autoFilter ref="D2:G3"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{1CAFD6A5-0771-4D4F-B29C-8C8A4BD59DAD}" name="DAYS"/>
-    <tableColumn id="2" xr3:uid="{D6E424DD-7C72-4461-BBE2-CD59B37123B3}" name="HOURS"/>
-    <tableColumn id="3" xr3:uid="{20858E5D-6D7D-4382-8DBC-1FD4091C418E}" name="MINUTES"/>
-    <tableColumn id="4" xr3:uid="{7FA7784E-0318-4F9C-9B40-57F4F3F3FD45}" name="EQUIVALENT HOURS" dataDxfId="5">
+    <tableColumn id="1" name="DAYS"/>
+    <tableColumn id="2" name="HOURS"/>
+    <tableColumn id="3" name="MINUTES"/>
+    <tableColumn id="4" name="EQUIVALENT HOURS" dataDxfId="5">
       <calculatedColumnFormula>SUMIFS(F7:F14,E7:E14,E3)+SUMIFS(D7:D66,C7:C66,F3)+D3</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2607,14 +2602,14 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{CB4120CB-17DA-4A84-90C5-840D28205819}" name="Table3" displayName="Table3" ref="J2:L3" totalsRowShown="0" headerRowBorderDxfId="4" tableBorderDxfId="3">
-  <autoFilter ref="J2:L3" xr:uid="{CB4120CB-17DA-4A84-90C5-840D28205819}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="J2:L3" totalsRowShown="0" headerRowBorderDxfId="4" tableBorderDxfId="3">
+  <autoFilter ref="J2:L3"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{6D76F81F-2FB2-4658-9985-FB0CE23F1771}" name="DATE STARTED" dataDxfId="2"/>
-    <tableColumn id="2" xr3:uid="{40B8C089-638A-4D13-9FCC-740888AE7704}" name="LEAVE EARN" dataDxfId="1">
+    <tableColumn id="1" name="DATE STARTED" dataDxfId="2"/>
+    <tableColumn id="2" name="LEAVE EARN" dataDxfId="1">
       <calculatedColumnFormula>J4-1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{C3A40ACA-C07A-4798-82C2-714BDF47B4DB}" name="LEAVE EARNED" dataDxfId="0">
+    <tableColumn id="3" name="LEAVE EARNED" dataDxfId="0">
       <calculatedColumnFormula>IF($J$4=1,1.25,IF(ISBLANK($J$3),"---",1.25-VLOOKUP($K$3,$I$8:$K$37,2)))</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2918,7 +2913,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D098C40-D36A-4A12-B6E1-6D049DE49862}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1">
     <tabColor rgb="FFFF0000"/>
   </sheetPr>
@@ -2928,7 +2923,7 @@
       <selection activeCell="Z62" sqref="Z62"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -2936,34 +2931,34 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0FF8E2B-FA0C-43AD-94F6-3305AF75672F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A2:K130"/>
+  <dimension ref="A2:K117"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="5520" topLeftCell="A34" activePane="bottomLeft"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="60" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="2070" topLeftCell="A9" activePane="bottomLeft"/>
       <selection activeCell="B4" sqref="B4:C4"/>
-      <selection pane="bottomLeft" activeCell="N14" sqref="N14"/>
+      <selection pane="bottomLeft" activeCell="S114" sqref="S114"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.33203125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="16.5546875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="12.109375" style="30" customWidth="1"/>
-    <col min="4" max="4" width="12.6640625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="11.77734375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="12.6640625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="12.109375" style="30" customWidth="1"/>
-    <col min="8" max="8" width="12.6640625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="11.77734375" style="1" customWidth="1"/>
-    <col min="10" max="10" width="12.6640625" style="1" customWidth="1"/>
-    <col min="11" max="11" width="24.88671875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="10.28515625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="16.5703125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" style="30" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="11.7109375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="12.7109375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="12.140625" style="30" customWidth="1"/>
+    <col min="8" max="8" width="12.7109375" style="1" customWidth="1"/>
+    <col min="9" max="9" width="11.7109375" style="1" customWidth="1"/>
+    <col min="10" max="10" width="12.7109375" style="1" customWidth="1"/>
+    <col min="11" max="11" width="24.85546875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:11" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" ht="20.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="29" t="s">
         <v>9</v>
       </c>
@@ -2982,7 +2977,7 @@
       <c r="J2" s="50"/>
       <c r="K2" s="51"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="18" t="s">
         <v>15</v>
       </c>
@@ -3000,7 +2995,7 @@
       <c r="J3" s="52"/>
       <c r="K3" s="53"/>
     </row>
-    <row r="4" spans="1:11" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="18" t="s">
         <v>16</v>
       </c>
@@ -3018,7 +3013,7 @@
       <c r="J4" s="54"/>
       <c r="K4" s="55"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="16"/>
       <c r="H5" s="27" t="s">
         <v>18</v>
@@ -3026,7 +3021,7 @@
       <c r="I5" s="27"/>
       <c r="K5" s="4"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="17"/>
       <c r="B6" s="8"/>
       <c r="C6" s="31"/>
@@ -3039,7 +3034,7 @@
       <c r="J6" s="8"/>
       <c r="K6" s="19"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="14"/>
       <c r="B7" s="14"/>
       <c r="C7" s="48" t="s">
@@ -3056,7 +3051,7 @@
       <c r="J7" s="48"/>
       <c r="K7" s="14"/>
     </row>
-    <row r="8" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>0</v>
       </c>
@@ -3091,7 +3086,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="23"/>
       <c r="B9" s="24" t="s">
         <v>23</v>
@@ -3115,7 +3110,7 @@
       <c r="J9" s="11"/>
       <c r="K9" s="20"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="40"/>
       <c r="B10" s="20"/>
       <c r="C10" s="13"/>
@@ -3135,7 +3130,7 @@
       <c r="J10" s="11"/>
       <c r="K10" s="20"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="40"/>
       <c r="B11" s="20"/>
       <c r="C11" s="13"/>
@@ -3151,7 +3146,7 @@
       <c r="J11" s="11"/>
       <c r="K11" s="20"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="40"/>
       <c r="B12" s="20"/>
       <c r="C12" s="13"/>
@@ -3167,7 +3162,7 @@
       <c r="J12" s="11"/>
       <c r="K12" s="20"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="40"/>
       <c r="B13" s="20"/>
       <c r="C13" s="13"/>
@@ -3183,7 +3178,7 @@
       <c r="J13" s="11"/>
       <c r="K13" s="20"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="40"/>
       <c r="B14" s="20"/>
       <c r="C14" s="13"/>
@@ -3199,7 +3194,7 @@
       <c r="J14" s="11"/>
       <c r="K14" s="20"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="40"/>
       <c r="B15" s="20"/>
       <c r="C15" s="13"/>
@@ -3215,7 +3210,7 @@
       <c r="J15" s="11"/>
       <c r="K15" s="20"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="41"/>
       <c r="B16" s="15"/>
       <c r="C16" s="42"/>
@@ -3231,7 +3226,7 @@
       <c r="J16" s="12"/>
       <c r="K16" s="15"/>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="40"/>
       <c r="B17" s="20"/>
       <c r="C17" s="13"/>
@@ -3247,7 +3242,7 @@
       <c r="J17" s="11"/>
       <c r="K17" s="20"/>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="40"/>
       <c r="B18" s="20"/>
       <c r="C18" s="13"/>
@@ -3263,7 +3258,7 @@
       <c r="J18" s="11"/>
       <c r="K18" s="20"/>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="40"/>
       <c r="B19" s="20"/>
       <c r="C19" s="13"/>
@@ -3279,7 +3274,7 @@
       <c r="J19" s="11"/>
       <c r="K19" s="20"/>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="40"/>
       <c r="B20" s="20"/>
       <c r="C20" s="13"/>
@@ -3295,7 +3290,7 @@
       <c r="J20" s="11"/>
       <c r="K20" s="20"/>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="40"/>
       <c r="B21" s="20"/>
       <c r="C21" s="13"/>
@@ -3311,7 +3306,7 @@
       <c r="J21" s="11"/>
       <c r="K21" s="20"/>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="40"/>
       <c r="B22" s="20"/>
       <c r="C22" s="13"/>
@@ -3327,7 +3322,7 @@
       <c r="J22" s="11"/>
       <c r="K22" s="20"/>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="40"/>
       <c r="B23" s="20"/>
       <c r="C23" s="13"/>
@@ -3343,7 +3338,7 @@
       <c r="J23" s="11"/>
       <c r="K23" s="20"/>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="40"/>
       <c r="B24" s="20"/>
       <c r="C24" s="13"/>
@@ -3359,7 +3354,7 @@
       <c r="J24" s="11"/>
       <c r="K24" s="20"/>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="40"/>
       <c r="B25" s="20"/>
       <c r="C25" s="13"/>
@@ -3375,7 +3370,7 @@
       <c r="J25" s="11"/>
       <c r="K25" s="20"/>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="40"/>
       <c r="B26" s="20"/>
       <c r="C26" s="13"/>
@@ -3391,7 +3386,7 @@
       <c r="J26" s="11"/>
       <c r="K26" s="20"/>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="40"/>
       <c r="B27" s="20"/>
       <c r="C27" s="13"/>
@@ -3407,7 +3402,7 @@
       <c r="J27" s="11"/>
       <c r="K27" s="20"/>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="40"/>
       <c r="B28" s="20"/>
       <c r="C28" s="13"/>
@@ -3423,7 +3418,7 @@
       <c r="J28" s="11"/>
       <c r="K28" s="20"/>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="40"/>
       <c r="B29" s="20"/>
       <c r="C29" s="13"/>
@@ -3439,7 +3434,7 @@
       <c r="J29" s="11"/>
       <c r="K29" s="20"/>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="40"/>
       <c r="B30" s="20"/>
       <c r="C30" s="13"/>
@@ -3455,7 +3450,7 @@
       <c r="J30" s="11"/>
       <c r="K30" s="20"/>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="40"/>
       <c r="B31" s="20"/>
       <c r="C31" s="13"/>
@@ -3471,7 +3466,7 @@
       <c r="J31" s="11"/>
       <c r="K31" s="20"/>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="40"/>
       <c r="B32" s="20"/>
       <c r="C32" s="13"/>
@@ -3487,7 +3482,7 @@
       <c r="J32" s="11"/>
       <c r="K32" s="20"/>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" s="40"/>
       <c r="B33" s="20"/>
       <c r="C33" s="13"/>
@@ -3503,7 +3498,7 @@
       <c r="J33" s="11"/>
       <c r="K33" s="20"/>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" s="40"/>
       <c r="B34" s="20"/>
       <c r="C34" s="13"/>
@@ -3519,7 +3514,7 @@
       <c r="J34" s="11"/>
       <c r="K34" s="20"/>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" s="40"/>
       <c r="B35" s="20"/>
       <c r="C35" s="13"/>
@@ -3535,7 +3530,7 @@
       <c r="J35" s="11"/>
       <c r="K35" s="20"/>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" s="40"/>
       <c r="B36" s="20"/>
       <c r="C36" s="13"/>
@@ -3551,7 +3546,7 @@
       <c r="J36" s="11"/>
       <c r="K36" s="20"/>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" s="40"/>
       <c r="B37" s="20"/>
       <c r="C37" s="13"/>
@@ -3567,7 +3562,7 @@
       <c r="J37" s="11"/>
       <c r="K37" s="20"/>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" s="40"/>
       <c r="B38" s="20"/>
       <c r="C38" s="13"/>
@@ -3583,7 +3578,7 @@
       <c r="J38" s="11"/>
       <c r="K38" s="20"/>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" s="40"/>
       <c r="B39" s="20"/>
       <c r="C39" s="13"/>
@@ -3599,7 +3594,7 @@
       <c r="J39" s="11"/>
       <c r="K39" s="20"/>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" s="40"/>
       <c r="B40" s="20"/>
       <c r="C40" s="13"/>
@@ -3615,7 +3610,7 @@
       <c r="J40" s="11"/>
       <c r="K40" s="20"/>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" s="40"/>
       <c r="B41" s="20"/>
       <c r="C41" s="13"/>
@@ -3631,7 +3626,7 @@
       <c r="J41" s="11"/>
       <c r="K41" s="20"/>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" s="40"/>
       <c r="B42" s="20"/>
       <c r="C42" s="13"/>
@@ -3647,7 +3642,7 @@
       <c r="J42" s="11"/>
       <c r="K42" s="20"/>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" s="40"/>
       <c r="B43" s="20"/>
       <c r="C43" s="13"/>
@@ -3663,7 +3658,7 @@
       <c r="J43" s="11"/>
       <c r="K43" s="20"/>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" s="40"/>
       <c r="B44" s="20"/>
       <c r="C44" s="13"/>
@@ -3679,7 +3674,7 @@
       <c r="J44" s="11"/>
       <c r="K44" s="20"/>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" s="40"/>
       <c r="B45" s="20"/>
       <c r="C45" s="13"/>
@@ -3695,7 +3690,7 @@
       <c r="J45" s="11"/>
       <c r="K45" s="20"/>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" s="40"/>
       <c r="B46" s="20"/>
       <c r="C46" s="13"/>
@@ -3711,7 +3706,7 @@
       <c r="J46" s="11"/>
       <c r="K46" s="20"/>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47" s="40"/>
       <c r="B47" s="20"/>
       <c r="C47" s="13"/>
@@ -3727,7 +3722,7 @@
       <c r="J47" s="11"/>
       <c r="K47" s="20"/>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48" s="40"/>
       <c r="B48" s="20"/>
       <c r="C48" s="13"/>
@@ -3743,7 +3738,7 @@
       <c r="J48" s="11"/>
       <c r="K48" s="20"/>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49" s="40"/>
       <c r="B49" s="20"/>
       <c r="C49" s="13"/>
@@ -3759,7 +3754,7 @@
       <c r="J49" s="11"/>
       <c r="K49" s="20"/>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50" s="40"/>
       <c r="B50" s="20"/>
       <c r="C50" s="13"/>
@@ -3775,7 +3770,7 @@
       <c r="J50" s="11"/>
       <c r="K50" s="20"/>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51" s="40"/>
       <c r="B51" s="20"/>
       <c r="C51" s="13"/>
@@ -3791,7 +3786,7 @@
       <c r="J51" s="11"/>
       <c r="K51" s="20"/>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52" s="40"/>
       <c r="B52" s="20"/>
       <c r="C52" s="13"/>
@@ -3807,7 +3802,7 @@
       <c r="J52" s="11"/>
       <c r="K52" s="20"/>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53" s="40"/>
       <c r="B53" s="20"/>
       <c r="C53" s="13"/>
@@ -3823,7 +3818,7 @@
       <c r="J53" s="11"/>
       <c r="K53" s="20"/>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A54" s="40"/>
       <c r="B54" s="20"/>
       <c r="C54" s="13"/>
@@ -3839,7 +3834,7 @@
       <c r="J54" s="11"/>
       <c r="K54" s="20"/>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A55" s="40"/>
       <c r="B55" s="20"/>
       <c r="C55" s="13"/>
@@ -3855,7 +3850,7 @@
       <c r="J55" s="11"/>
       <c r="K55" s="20"/>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A56" s="40"/>
       <c r="B56" s="20"/>
       <c r="C56" s="13"/>
@@ -3871,7 +3866,7 @@
       <c r="J56" s="11"/>
       <c r="K56" s="20"/>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A57" s="40"/>
       <c r="B57" s="20"/>
       <c r="C57" s="13"/>
@@ -3887,7 +3882,7 @@
       <c r="J57" s="11"/>
       <c r="K57" s="20"/>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A58" s="40"/>
       <c r="B58" s="20"/>
       <c r="C58" s="13"/>
@@ -3903,7 +3898,7 @@
       <c r="J58" s="11"/>
       <c r="K58" s="20"/>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A59" s="40"/>
       <c r="B59" s="20"/>
       <c r="C59" s="13"/>
@@ -3919,7 +3914,7 @@
       <c r="J59" s="11"/>
       <c r="K59" s="20"/>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A60" s="40"/>
       <c r="B60" s="20"/>
       <c r="C60" s="13"/>
@@ -3935,7 +3930,7 @@
       <c r="J60" s="11"/>
       <c r="K60" s="20"/>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A61" s="40"/>
       <c r="B61" s="20"/>
       <c r="C61" s="13"/>
@@ -3951,7 +3946,7 @@
       <c r="J61" s="11"/>
       <c r="K61" s="20"/>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A62" s="40"/>
       <c r="B62" s="20"/>
       <c r="C62" s="13"/>
@@ -3967,7 +3962,7 @@
       <c r="J62" s="11"/>
       <c r="K62" s="20"/>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A63" s="40"/>
       <c r="B63" s="20"/>
       <c r="C63" s="13"/>
@@ -3983,7 +3978,7 @@
       <c r="J63" s="11"/>
       <c r="K63" s="20"/>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A64" s="40"/>
       <c r="B64" s="20"/>
       <c r="C64" s="13"/>
@@ -3999,7 +3994,7 @@
       <c r="J64" s="11"/>
       <c r="K64" s="20"/>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A65" s="40"/>
       <c r="B65" s="20"/>
       <c r="C65" s="13"/>
@@ -4015,7 +4010,7 @@
       <c r="J65" s="11"/>
       <c r="K65" s="20"/>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A66" s="40"/>
       <c r="B66" s="20"/>
       <c r="C66" s="13"/>
@@ -4031,7 +4026,7 @@
       <c r="J66" s="11"/>
       <c r="K66" s="20"/>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A67" s="40"/>
       <c r="B67" s="20"/>
       <c r="C67" s="13"/>
@@ -4047,7 +4042,7 @@
       <c r="J67" s="11"/>
       <c r="K67" s="20"/>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A68" s="40"/>
       <c r="B68" s="20"/>
       <c r="C68" s="13"/>
@@ -4063,7 +4058,7 @@
       <c r="J68" s="11"/>
       <c r="K68" s="20"/>
     </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A69" s="40"/>
       <c r="B69" s="20"/>
       <c r="C69" s="13"/>
@@ -4079,7 +4074,7 @@
       <c r="J69" s="11"/>
       <c r="K69" s="20"/>
     </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A70" s="40"/>
       <c r="B70" s="20"/>
       <c r="C70" s="13"/>
@@ -4095,7 +4090,7 @@
       <c r="J70" s="11"/>
       <c r="K70" s="20"/>
     </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A71" s="40"/>
       <c r="B71" s="20"/>
       <c r="C71" s="13"/>
@@ -4111,7 +4106,7 @@
       <c r="J71" s="11"/>
       <c r="K71" s="20"/>
     </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A72" s="40"/>
       <c r="B72" s="20"/>
       <c r="C72" s="13"/>
@@ -4127,7 +4122,7 @@
       <c r="J72" s="11"/>
       <c r="K72" s="20"/>
     </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A73" s="40"/>
       <c r="B73" s="20"/>
       <c r="C73" s="13"/>
@@ -4143,7 +4138,7 @@
       <c r="J73" s="11"/>
       <c r="K73" s="20"/>
     </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A74" s="40"/>
       <c r="B74" s="20"/>
       <c r="C74" s="13"/>
@@ -4159,7 +4154,7 @@
       <c r="J74" s="11"/>
       <c r="K74" s="20"/>
     </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A75" s="40"/>
       <c r="B75" s="20"/>
       <c r="C75" s="13"/>
@@ -4175,7 +4170,7 @@
       <c r="J75" s="11"/>
       <c r="K75" s="20"/>
     </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A76" s="40"/>
       <c r="B76" s="20"/>
       <c r="C76" s="13"/>
@@ -4191,7 +4186,7 @@
       <c r="J76" s="11"/>
       <c r="K76" s="20"/>
     </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A77" s="40"/>
       <c r="B77" s="20"/>
       <c r="C77" s="13"/>
@@ -4207,7 +4202,7 @@
       <c r="J77" s="11"/>
       <c r="K77" s="20"/>
     </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A78" s="40"/>
       <c r="B78" s="20"/>
       <c r="C78" s="13"/>
@@ -4223,7 +4218,7 @@
       <c r="J78" s="11"/>
       <c r="K78" s="20"/>
     </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A79" s="40"/>
       <c r="B79" s="20"/>
       <c r="C79" s="13"/>
@@ -4239,7 +4234,7 @@
       <c r="J79" s="11"/>
       <c r="K79" s="20"/>
     </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A80" s="40"/>
       <c r="B80" s="20"/>
       <c r="C80" s="13"/>
@@ -4255,7 +4250,7 @@
       <c r="J80" s="11"/>
       <c r="K80" s="20"/>
     </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A81" s="40"/>
       <c r="B81" s="20"/>
       <c r="C81" s="13"/>
@@ -4271,7 +4266,7 @@
       <c r="J81" s="11"/>
       <c r="K81" s="20"/>
     </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A82" s="40"/>
       <c r="B82" s="20"/>
       <c r="C82" s="13"/>
@@ -4287,7 +4282,7 @@
       <c r="J82" s="11"/>
       <c r="K82" s="20"/>
     </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A83" s="40"/>
       <c r="B83" s="20"/>
       <c r="C83" s="13"/>
@@ -4303,7 +4298,7 @@
       <c r="J83" s="11"/>
       <c r="K83" s="20"/>
     </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A84" s="40"/>
       <c r="B84" s="20"/>
       <c r="C84" s="13"/>
@@ -4319,7 +4314,7 @@
       <c r="J84" s="11"/>
       <c r="K84" s="20"/>
     </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A85" s="40"/>
       <c r="B85" s="20"/>
       <c r="C85" s="13"/>
@@ -4335,7 +4330,7 @@
       <c r="J85" s="11"/>
       <c r="K85" s="20"/>
     </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A86" s="40"/>
       <c r="B86" s="20"/>
       <c r="C86" s="13"/>
@@ -4351,7 +4346,7 @@
       <c r="J86" s="11"/>
       <c r="K86" s="20"/>
     </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A87" s="40"/>
       <c r="B87" s="20"/>
       <c r="C87" s="13"/>
@@ -4367,7 +4362,7 @@
       <c r="J87" s="11"/>
       <c r="K87" s="20"/>
     </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A88" s="40"/>
       <c r="B88" s="20"/>
       <c r="C88" s="13"/>
@@ -4383,7 +4378,7 @@
       <c r="J88" s="11"/>
       <c r="K88" s="20"/>
     </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A89" s="40"/>
       <c r="B89" s="20"/>
       <c r="C89" s="13"/>
@@ -4399,7 +4394,7 @@
       <c r="J89" s="11"/>
       <c r="K89" s="20"/>
     </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A90" s="40"/>
       <c r="B90" s="20"/>
       <c r="C90" s="13"/>
@@ -4415,7 +4410,7 @@
       <c r="J90" s="11"/>
       <c r="K90" s="20"/>
     </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A91" s="40"/>
       <c r="B91" s="20"/>
       <c r="C91" s="13"/>
@@ -4431,7 +4426,7 @@
       <c r="J91" s="11"/>
       <c r="K91" s="20"/>
     </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A92" s="40"/>
       <c r="B92" s="20"/>
       <c r="C92" s="13"/>
@@ -4447,7 +4442,7 @@
       <c r="J92" s="11"/>
       <c r="K92" s="20"/>
     </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A93" s="40"/>
       <c r="B93" s="20"/>
       <c r="C93" s="13"/>
@@ -4463,7 +4458,7 @@
       <c r="J93" s="11"/>
       <c r="K93" s="20"/>
     </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A94" s="40"/>
       <c r="B94" s="20"/>
       <c r="C94" s="13"/>
@@ -4479,7 +4474,7 @@
       <c r="J94" s="11"/>
       <c r="K94" s="20"/>
     </row>
-    <row r="95" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A95" s="40"/>
       <c r="B95" s="20"/>
       <c r="C95" s="13"/>
@@ -4495,7 +4490,7 @@
       <c r="J95" s="11"/>
       <c r="K95" s="20"/>
     </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A96" s="40"/>
       <c r="B96" s="20"/>
       <c r="C96" s="13"/>
@@ -4511,7 +4506,7 @@
       <c r="J96" s="11"/>
       <c r="K96" s="20"/>
     </row>
-    <row r="97" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A97" s="40"/>
       <c r="B97" s="20"/>
       <c r="C97" s="13"/>
@@ -4527,7 +4522,7 @@
       <c r="J97" s="11"/>
       <c r="K97" s="20"/>
     </row>
-    <row r="98" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A98" s="40"/>
       <c r="B98" s="20"/>
       <c r="C98" s="13"/>
@@ -4543,7 +4538,7 @@
       <c r="J98" s="11"/>
       <c r="K98" s="20"/>
     </row>
-    <row r="99" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A99" s="40"/>
       <c r="B99" s="20"/>
       <c r="C99" s="13"/>
@@ -4559,7 +4554,7 @@
       <c r="J99" s="11"/>
       <c r="K99" s="20"/>
     </row>
-    <row r="100" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A100" s="40"/>
       <c r="B100" s="20"/>
       <c r="C100" s="13"/>
@@ -4575,7 +4570,7 @@
       <c r="J100" s="11"/>
       <c r="K100" s="20"/>
     </row>
-    <row r="101" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A101" s="40"/>
       <c r="B101" s="20"/>
       <c r="C101" s="13"/>
@@ -4591,7 +4586,7 @@
       <c r="J101" s="11"/>
       <c r="K101" s="20"/>
     </row>
-    <row r="102" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A102" s="40"/>
       <c r="B102" s="20"/>
       <c r="C102" s="13"/>
@@ -4607,7 +4602,7 @@
       <c r="J102" s="11"/>
       <c r="K102" s="20"/>
     </row>
-    <row r="103" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A103" s="40"/>
       <c r="B103" s="20"/>
       <c r="C103" s="13"/>
@@ -4623,7 +4618,7 @@
       <c r="J103" s="11"/>
       <c r="K103" s="20"/>
     </row>
-    <row r="104" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A104" s="40"/>
       <c r="B104" s="20"/>
       <c r="C104" s="13"/>
@@ -4639,7 +4634,7 @@
       <c r="J104" s="11"/>
       <c r="K104" s="20"/>
     </row>
-    <row r="105" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A105" s="40"/>
       <c r="B105" s="20"/>
       <c r="C105" s="13"/>
@@ -4655,7 +4650,7 @@
       <c r="J105" s="11"/>
       <c r="K105" s="20"/>
     </row>
-    <row r="106" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A106" s="40"/>
       <c r="B106" s="20"/>
       <c r="C106" s="13"/>
@@ -4671,7 +4666,7 @@
       <c r="J106" s="11"/>
       <c r="K106" s="20"/>
     </row>
-    <row r="107" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A107" s="40"/>
       <c r="B107" s="20"/>
       <c r="C107" s="13"/>
@@ -4687,7 +4682,7 @@
       <c r="J107" s="11"/>
       <c r="K107" s="20"/>
     </row>
-    <row r="108" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A108" s="40"/>
       <c r="B108" s="20"/>
       <c r="C108" s="13"/>
@@ -4703,7 +4698,7 @@
       <c r="J108" s="11"/>
       <c r="K108" s="20"/>
     </row>
-    <row r="109" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A109" s="40"/>
       <c r="B109" s="20"/>
       <c r="C109" s="13"/>
@@ -4719,7 +4714,7 @@
       <c r="J109" s="11"/>
       <c r="K109" s="20"/>
     </row>
-    <row r="110" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A110" s="40"/>
       <c r="B110" s="20"/>
       <c r="C110" s="13"/>
@@ -4735,7 +4730,7 @@
       <c r="J110" s="11"/>
       <c r="K110" s="20"/>
     </row>
-    <row r="111" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A111" s="40"/>
       <c r="B111" s="20"/>
       <c r="C111" s="13"/>
@@ -4751,7 +4746,7 @@
       <c r="J111" s="11"/>
       <c r="K111" s="20"/>
     </row>
-    <row r="112" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A112" s="40"/>
       <c r="B112" s="20"/>
       <c r="C112" s="13"/>
@@ -4767,7 +4762,7 @@
       <c r="J112" s="11"/>
       <c r="K112" s="20"/>
     </row>
-    <row r="113" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A113" s="40"/>
       <c r="B113" s="20"/>
       <c r="C113" s="13"/>
@@ -4783,7 +4778,7 @@
       <c r="J113" s="11"/>
       <c r="K113" s="20"/>
     </row>
-    <row r="114" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A114" s="40"/>
       <c r="B114" s="20"/>
       <c r="C114" s="13"/>
@@ -4799,7 +4794,7 @@
       <c r="J114" s="11"/>
       <c r="K114" s="20"/>
     </row>
-    <row r="115" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A115" s="40"/>
       <c r="B115" s="20"/>
       <c r="C115" s="13"/>
@@ -4815,7 +4810,7 @@
       <c r="J115" s="11"/>
       <c r="K115" s="20"/>
     </row>
-    <row r="116" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A116" s="40"/>
       <c r="B116" s="20"/>
       <c r="C116" s="13"/>
@@ -4831,7 +4826,7 @@
       <c r="J116" s="11"/>
       <c r="K116" s="20"/>
     </row>
-    <row r="117" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A117" s="40"/>
       <c r="B117" s="20"/>
       <c r="C117" s="13"/>
@@ -4846,214 +4841,6 @@
       <c r="I117" s="9"/>
       <c r="J117" s="11"/>
       <c r="K117" s="20"/>
-    </row>
-    <row r="118" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A118" s="40"/>
-      <c r="B118" s="20"/>
-      <c r="C118" s="13"/>
-      <c r="D118" s="39"/>
-      <c r="E118" s="9"/>
-      <c r="F118" s="20"/>
-      <c r="G118" s="13" t="str">
-        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
-        <v/>
-      </c>
-      <c r="H118" s="39"/>
-      <c r="I118" s="9"/>
-      <c r="J118" s="11"/>
-      <c r="K118" s="20"/>
-    </row>
-    <row r="119" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A119" s="40"/>
-      <c r="B119" s="20"/>
-      <c r="C119" s="13"/>
-      <c r="D119" s="39"/>
-      <c r="E119" s="9"/>
-      <c r="F119" s="20"/>
-      <c r="G119" s="13" t="str">
-        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
-        <v/>
-      </c>
-      <c r="H119" s="39"/>
-      <c r="I119" s="9"/>
-      <c r="J119" s="11"/>
-      <c r="K119" s="20"/>
-    </row>
-    <row r="120" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A120" s="40"/>
-      <c r="B120" s="20"/>
-      <c r="C120" s="13"/>
-      <c r="D120" s="39"/>
-      <c r="E120" s="9"/>
-      <c r="F120" s="20"/>
-      <c r="G120" s="13" t="str">
-        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
-        <v/>
-      </c>
-      <c r="H120" s="39"/>
-      <c r="I120" s="9"/>
-      <c r="J120" s="11"/>
-      <c r="K120" s="20"/>
-    </row>
-    <row r="121" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A121" s="40"/>
-      <c r="B121" s="20"/>
-      <c r="C121" s="13"/>
-      <c r="D121" s="39"/>
-      <c r="E121" s="9"/>
-      <c r="F121" s="20"/>
-      <c r="G121" s="13" t="str">
-        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
-        <v/>
-      </c>
-      <c r="H121" s="39"/>
-      <c r="I121" s="9"/>
-      <c r="J121" s="11"/>
-      <c r="K121" s="20"/>
-    </row>
-    <row r="122" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A122" s="40"/>
-      <c r="B122" s="20"/>
-      <c r="C122" s="13"/>
-      <c r="D122" s="39"/>
-      <c r="E122" s="9"/>
-      <c r="F122" s="20"/>
-      <c r="G122" s="13" t="str">
-        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
-        <v/>
-      </c>
-      <c r="H122" s="39"/>
-      <c r="I122" s="9"/>
-      <c r="J122" s="11"/>
-      <c r="K122" s="20"/>
-    </row>
-    <row r="123" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A123" s="40"/>
-      <c r="B123" s="20"/>
-      <c r="C123" s="13"/>
-      <c r="D123" s="39"/>
-      <c r="E123" s="9"/>
-      <c r="F123" s="20"/>
-      <c r="G123" s="13" t="str">
-        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
-        <v/>
-      </c>
-      <c r="H123" s="39"/>
-      <c r="I123" s="9"/>
-      <c r="J123" s="11"/>
-      <c r="K123" s="20"/>
-    </row>
-    <row r="124" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A124" s="40"/>
-      <c r="B124" s="20"/>
-      <c r="C124" s="13"/>
-      <c r="D124" s="39"/>
-      <c r="E124" s="9"/>
-      <c r="F124" s="20"/>
-      <c r="G124" s="13" t="str">
-        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
-        <v/>
-      </c>
-      <c r="H124" s="39"/>
-      <c r="I124" s="9"/>
-      <c r="J124" s="11"/>
-      <c r="K124" s="20"/>
-    </row>
-    <row r="125" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A125" s="40"/>
-      <c r="B125" s="20"/>
-      <c r="C125" s="13"/>
-      <c r="D125" s="39"/>
-      <c r="E125" s="9"/>
-      <c r="F125" s="20"/>
-      <c r="G125" s="13" t="str">
-        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
-        <v/>
-      </c>
-      <c r="H125" s="39"/>
-      <c r="I125" s="9"/>
-      <c r="J125" s="11"/>
-      <c r="K125" s="20"/>
-    </row>
-    <row r="126" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A126" s="40"/>
-      <c r="B126" s="20"/>
-      <c r="C126" s="13"/>
-      <c r="D126" s="39"/>
-      <c r="E126" s="9"/>
-      <c r="F126" s="20"/>
-      <c r="G126" s="13" t="str">
-        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
-        <v/>
-      </c>
-      <c r="H126" s="39"/>
-      <c r="I126" s="9"/>
-      <c r="J126" s="11"/>
-      <c r="K126" s="20"/>
-    </row>
-    <row r="127" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A127" s="40"/>
-      <c r="B127" s="20"/>
-      <c r="C127" s="13"/>
-      <c r="D127" s="39"/>
-      <c r="E127" s="9"/>
-      <c r="F127" s="20"/>
-      <c r="G127" s="13" t="str">
-        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
-        <v/>
-      </c>
-      <c r="H127" s="39"/>
-      <c r="I127" s="9"/>
-      <c r="J127" s="11"/>
-      <c r="K127" s="20"/>
-    </row>
-    <row r="128" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A128" s="40"/>
-      <c r="B128" s="20"/>
-      <c r="C128" s="13"/>
-      <c r="D128" s="39"/>
-      <c r="E128" s="9"/>
-      <c r="F128" s="20"/>
-      <c r="G128" s="13" t="str">
-        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
-        <v/>
-      </c>
-      <c r="H128" s="39"/>
-      <c r="I128" s="9"/>
-      <c r="J128" s="11"/>
-      <c r="K128" s="20"/>
-    </row>
-    <row r="129" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A129" s="40"/>
-      <c r="B129" s="20"/>
-      <c r="C129" s="13"/>
-      <c r="D129" s="39"/>
-      <c r="E129" s="9"/>
-      <c r="F129" s="20"/>
-      <c r="G129" s="13" t="str">
-        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
-        <v/>
-      </c>
-      <c r="H129" s="39"/>
-      <c r="I129" s="9"/>
-      <c r="J129" s="11"/>
-      <c r="K129" s="20"/>
-    </row>
-    <row r="130" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A130" s="41"/>
-      <c r="B130" s="15"/>
-      <c r="C130" s="42"/>
-      <c r="D130" s="43"/>
-      <c r="E130" s="9"/>
-      <c r="F130" s="15"/>
-      <c r="G130" s="42" t="str">
-        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
-        <v/>
-      </c>
-      <c r="H130" s="43"/>
-      <c r="I130" s="9"/>
-      <c r="J130" s="12"/>
-      <c r="K130" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="11">
@@ -5070,10 +4857,10 @@
     <mergeCell ref="F4:G4"/>
   </mergeCells>
   <dataValidations disablePrompts="1" count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:G2" xr:uid="{3C67B38A-DE91-4BA1-85D0-F5C61D6395E6}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:G2">
       <formula1>"1 - Married (and not separated), 2 - Widowed (including living common law), 3 - Separated (including living common law), 4 - Divorced (including living common law), 5 - Single (including living common law)"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4:C4" xr:uid="{C9F25C0C-606E-415B-87B4-B098DE141EB5}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4:C4">
       <formula1>"PERMANENT, CO-TERMINUS, CASUAL, JOBCON"</formula1>
     </dataValidation>
   </dataValidations>
@@ -5096,7 +4883,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1CB8F789-193C-43F9-8D48-B0DEE5C76ADA}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:L67"/>
   <sheetViews>
@@ -5104,21 +4891,21 @@
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.21875" customWidth="1"/>
-    <col min="2" max="2" width="20.77734375" customWidth="1"/>
-    <col min="4" max="4" width="15.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="26.109375" customWidth="1"/>
-    <col min="9" max="9" width="16.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.33203125" customWidth="1"/>
-    <col min="11" max="11" width="14.88671875" style="37" hidden="1" customWidth="1"/>
-    <col min="12" max="12" width="15.5546875" customWidth="1"/>
+    <col min="1" max="1" width="21.28515625" customWidth="1"/>
+    <col min="2" max="2" width="20.7109375" customWidth="1"/>
+    <col min="4" max="4" width="15.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="26.140625" customWidth="1"/>
+    <col min="9" max="9" width="16.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.28515625" customWidth="1"/>
+    <col min="11" max="11" width="14.85546875" style="37" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="15.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D1" s="58" t="s">
         <v>33</v>
       </c>
@@ -5131,7 +4918,7 @@
       <c r="K1" s="59"/>
       <c r="L1" s="59"/>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="32" t="s">
         <v>24</v>
       </c>
@@ -5160,7 +4947,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="9">
         <f>Sheet1!E9</f>
         <v>0</v>
@@ -5186,17 +4973,17 @@
         <v>---</v>
       </c>
     </row>
-    <row r="4" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="G4" s="33"/>
       <c r="J4" s="1" t="str">
         <f>IF(TEXT(J3,"D")=1,1,TEXT(J3,"D"))</f>
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="J5" s="1"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>42</v>
       </c>
@@ -5220,7 +5007,7 @@
       <c r="K6" s="59"/>
       <c r="L6" s="59"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="9">
         <f>SUM(Sheet1!E9,Sheet1!I9)</f>
         <v>0</v>
@@ -5251,7 +5038,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C8" s="37">
         <v>2</v>
       </c>
@@ -5277,7 +5064,7 @@
         <v>4.2000000000000003E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C9" s="37">
         <v>3</v>
       </c>
@@ -5303,7 +5090,7 @@
         <v>8.3000000000000004E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C10" s="37">
         <v>4</v>
       </c>
@@ -5329,7 +5116,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C11" s="37">
         <v>5</v>
       </c>
@@ -5355,7 +5142,7 @@
         <v>0.16700000000000001</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C12" s="37">
         <v>6</v>
       </c>
@@ -5381,7 +5168,7 @@
         <v>0.20800000000000002</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C13" s="37">
         <v>7</v>
       </c>
@@ -5407,7 +5194,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C14" s="37">
         <v>8</v>
       </c>
@@ -5433,7 +5220,7 @@
         <v>0.29199999999999998</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C15" s="37">
         <v>9</v>
       </c>
@@ -5453,7 +5240,7 @@
         <v>0.33299999999999996</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C16" s="37">
         <v>10</v>
       </c>
@@ -5473,7 +5260,7 @@
         <v>0.37499999999999994</v>
       </c>
     </row>
-    <row r="17" spans="3:12" x14ac:dyDescent="0.3">
+    <row r="17" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C17" s="37">
         <v>11</v>
       </c>
@@ -5493,7 +5280,7 @@
         <v>0.41699999999999993</v>
       </c>
     </row>
-    <row r="18" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C18" s="37">
         <v>12</v>
       </c>
@@ -5514,7 +5301,7 @@
         <v>0.45799999999999991</v>
       </c>
     </row>
-    <row r="19" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C19" s="37">
         <v>13</v>
       </c>
@@ -5535,7 +5322,7 @@
         <v>0.49999999999999989</v>
       </c>
     </row>
-    <row r="20" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C20" s="37">
         <v>14</v>
       </c>
@@ -5556,7 +5343,7 @@
         <v>0.54199999999999993</v>
       </c>
     </row>
-    <row r="21" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C21" s="37">
         <v>15</v>
       </c>
@@ -5577,7 +5364,7 @@
         <v>0.58299999999999996</v>
       </c>
     </row>
-    <row r="22" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C22" s="37">
         <v>16</v>
       </c>
@@ -5598,7 +5385,7 @@
         <v>0.625</v>
       </c>
     </row>
-    <row r="23" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C23" s="37">
         <v>17</v>
       </c>
@@ -5619,7 +5406,7 @@
         <v>0.66700000000000004</v>
       </c>
     </row>
-    <row r="24" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C24" s="37">
         <v>18</v>
       </c>
@@ -5640,7 +5427,7 @@
         <v>0.70800000000000007</v>
       </c>
     </row>
-    <row r="25" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C25" s="37">
         <v>19</v>
       </c>
@@ -5661,7 +5448,7 @@
         <v>0.75000000000000011</v>
       </c>
     </row>
-    <row r="26" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C26" s="37">
         <v>20</v>
       </c>
@@ -5682,7 +5469,7 @@
         <v>0.79200000000000015</v>
       </c>
     </row>
-    <row r="27" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C27" s="37">
         <v>21</v>
       </c>
@@ -5703,7 +5490,7 @@
         <v>0.83300000000000018</v>
       </c>
     </row>
-    <row r="28" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C28" s="37">
         <v>22</v>
       </c>
@@ -5724,7 +5511,7 @@
         <v>0.87500000000000022</v>
       </c>
     </row>
-    <row r="29" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C29" s="37">
         <v>23</v>
       </c>
@@ -5745,7 +5532,7 @@
         <v>0.91700000000000026</v>
       </c>
     </row>
-    <row r="30" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C30" s="37">
         <v>24</v>
       </c>
@@ -5766,7 +5553,7 @@
         <v>0.9580000000000003</v>
       </c>
     </row>
-    <row r="31" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C31" s="37">
         <v>25</v>
       </c>
@@ -5787,7 +5574,7 @@
         <v>1.0000000000000002</v>
       </c>
     </row>
-    <row r="32" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C32" s="37">
         <v>26</v>
       </c>
@@ -5808,7 +5595,7 @@
         <v>1.0420000000000003</v>
       </c>
     </row>
-    <row r="33" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C33" s="37">
         <v>27</v>
       </c>
@@ -5829,7 +5616,7 @@
         <v>1.0830000000000002</v>
       </c>
     </row>
-    <row r="34" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C34" s="37">
         <v>28</v>
       </c>
@@ -5850,7 +5637,7 @@
         <v>1.1250000000000002</v>
       </c>
     </row>
-    <row r="35" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C35" s="37">
         <v>29</v>
       </c>
@@ -5871,7 +5658,7 @@
         <v>1.1670000000000003</v>
       </c>
     </row>
-    <row r="36" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C36" s="37">
         <v>30</v>
       </c>
@@ -5892,7 +5679,7 @@
         <v>1.2080000000000002</v>
       </c>
     </row>
-    <row r="37" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C37" s="37">
         <v>31</v>
       </c>
@@ -5913,7 +5700,7 @@
         <v>1.2500000000000002</v>
       </c>
     </row>
-    <row r="38" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C38" s="37">
         <v>32</v>
       </c>
@@ -5922,7 +5709,7 @@
       </c>
       <c r="G38"/>
     </row>
-    <row r="39" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C39" s="37">
         <v>33</v>
       </c>
@@ -5931,7 +5718,7 @@
       </c>
       <c r="G39"/>
     </row>
-    <row r="40" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C40" s="37">
         <v>34</v>
       </c>
@@ -5940,7 +5727,7 @@
       </c>
       <c r="G40"/>
     </row>
-    <row r="41" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C41" s="37">
         <v>35</v>
       </c>
@@ -5949,7 +5736,7 @@
       </c>
       <c r="G41"/>
     </row>
-    <row r="42" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C42" s="37">
         <v>36</v>
       </c>
@@ -5958,7 +5745,7 @@
       </c>
       <c r="G42"/>
     </row>
-    <row r="43" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C43" s="37">
         <v>37</v>
       </c>
@@ -5967,7 +5754,7 @@
       </c>
       <c r="G43"/>
     </row>
-    <row r="44" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C44" s="37">
         <v>38</v>
       </c>
@@ -5976,7 +5763,7 @@
       </c>
       <c r="G44"/>
     </row>
-    <row r="45" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C45" s="37">
         <v>39</v>
       </c>
@@ -5985,7 +5772,7 @@
       </c>
       <c r="G45"/>
     </row>
-    <row r="46" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C46" s="37">
         <v>40</v>
       </c>
@@ -5994,7 +5781,7 @@
       </c>
       <c r="G46"/>
     </row>
-    <row r="47" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C47" s="37">
         <v>41</v>
       </c>
@@ -6003,7 +5790,7 @@
       </c>
       <c r="G47"/>
     </row>
-    <row r="48" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C48" s="37">
         <v>42</v>
       </c>
@@ -6012,7 +5799,7 @@
       </c>
       <c r="G48"/>
     </row>
-    <row r="49" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C49" s="37">
         <v>43</v>
       </c>
@@ -6021,7 +5808,7 @@
       </c>
       <c r="G49"/>
     </row>
-    <row r="50" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C50" s="37">
         <v>44</v>
       </c>
@@ -6030,7 +5817,7 @@
       </c>
       <c r="G50"/>
     </row>
-    <row r="51" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C51" s="37">
         <v>45</v>
       </c>
@@ -6039,7 +5826,7 @@
       </c>
       <c r="G51"/>
     </row>
-    <row r="52" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C52" s="37">
         <v>46</v>
       </c>
@@ -6048,7 +5835,7 @@
       </c>
       <c r="G52"/>
     </row>
-    <row r="53" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C53" s="37">
         <v>47</v>
       </c>
@@ -6057,7 +5844,7 @@
       </c>
       <c r="G53"/>
     </row>
-    <row r="54" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C54" s="37">
         <v>48</v>
       </c>
@@ -6066,7 +5853,7 @@
       </c>
       <c r="G54"/>
     </row>
-    <row r="55" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C55" s="37">
         <v>49</v>
       </c>
@@ -6075,7 +5862,7 @@
       </c>
       <c r="G55"/>
     </row>
-    <row r="56" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C56" s="37">
         <v>50</v>
       </c>
@@ -6084,7 +5871,7 @@
       </c>
       <c r="G56"/>
     </row>
-    <row r="57" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C57" s="37">
         <v>51</v>
       </c>
@@ -6093,7 +5880,7 @@
       </c>
       <c r="G57"/>
     </row>
-    <row r="58" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C58" s="37">
         <v>52</v>
       </c>
@@ -6102,7 +5889,7 @@
       </c>
       <c r="G58"/>
     </row>
-    <row r="59" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C59" s="37">
         <v>53</v>
       </c>
@@ -6111,7 +5898,7 @@
       </c>
       <c r="G59"/>
     </row>
-    <row r="60" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C60" s="37">
         <v>54</v>
       </c>
@@ -6120,7 +5907,7 @@
       </c>
       <c r="G60"/>
     </row>
-    <row r="61" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C61" s="37">
         <v>55</v>
       </c>
@@ -6129,7 +5916,7 @@
       </c>
       <c r="G61"/>
     </row>
-    <row r="62" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C62" s="37">
         <v>56</v>
       </c>
@@ -6138,7 +5925,7 @@
       </c>
       <c r="G62"/>
     </row>
-    <row r="63" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C63" s="37">
         <v>57</v>
       </c>
@@ -6147,7 +5934,7 @@
       </c>
       <c r="G63"/>
     </row>
-    <row r="64" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C64" s="37">
         <v>58</v>
       </c>
@@ -6156,7 +5943,7 @@
       </c>
       <c r="G64"/>
     </row>
-    <row r="65" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C65" s="37">
         <v>59</v>
       </c>
@@ -6165,7 +5952,7 @@
       </c>
       <c r="G65"/>
     </row>
-    <row r="66" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C66" s="37">
         <v>60</v>
       </c>
@@ -6174,7 +5961,7 @@
       </c>
       <c r="G66"/>
     </row>
-    <row r="67" spans="3:12" x14ac:dyDescent="0.3">
+    <row r="67" spans="3:12" x14ac:dyDescent="0.25">
       <c r="J67" s="1"/>
       <c r="K67" s="1"/>
       <c r="L67" s="1"/>

</xml_diff>